<commit_message>
Audio board, one CAP20 package added
Audio release build
</commit_message>
<xml_diff>
--- a/V9.0/Audio - Routed - BOM.xlsx
+++ b/V9.0/Audio - Routed - BOM.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -10,9 +10,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A:$H</definedName>
-  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -23,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="145">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -52,9 +49,6 @@
     <t xml:space="preserve">Resistors</t>
   </si>
   <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
     <t xml:space="preserve">R1,R2,R4,R6,R8,R10,R12,R14,R16,R17,R18,R19,R21,R23,R25,R27,R29,R31,R33,R43,R44,R45,R46,R47,R48,R49,R50</t>
   </si>
   <si>
@@ -73,9 +67,6 @@
     <t xml:space="preserve">Top Copper</t>
   </si>
   <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
     <t xml:space="preserve">R3,R5,R7,R9,R11,R13,R15,R20,R22,R24,R26,R28,R30,R32,R34,R35,R36,R37,R38,R39,R42</t>
   </si>
   <si>
@@ -88,9 +79,6 @@
     <t xml:space="preserve">Integrated Circuits</t>
   </si>
   <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
     <t xml:space="preserve">U1,U7,U8,U19,U20,U26,U72,U204,U206,U207,U208</t>
   </si>
   <si>
@@ -106,9 +94,6 @@
     <t xml:space="preserve">DIL16CAP20</t>
   </si>
   <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
     <t xml:space="preserve">U2,U4,U6,U9,U14,U15,U77,U78,U79,U80,U85,U113,U114,U115,U116,U119,U153,U154,U155,U156,U159,U193,U194,U195,U196,U199</t>
   </si>
   <si>
@@ -124,9 +109,6 @@
     <t xml:space="preserve">DIL20CAP20</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
     <t xml:space="preserve">U3,U17,U122,U162,U202</t>
   </si>
   <si>
@@ -142,9 +124,6 @@
     <t xml:space="preserve">DIL14CAP20</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
     <t xml:space="preserve">U5</t>
   </si>
   <si>
@@ -157,9 +136,6 @@
     <t xml:space="preserve">Dual 4-Input Positive-AND Gates</t>
   </si>
   <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
     <t xml:space="preserve">U10,U11,U12,U13,U16,U18,U21,U88,U89,U98,U99,U100,U101,U129,U130,U138,U139,U140,U141,U169,U170,U178,U179,U180,U181</t>
   </si>
   <si>
@@ -172,9 +148,6 @@
     <t xml:space="preserve">Octal D-Type Positive-Edge-Triggered Flip-Flops With Clear</t>
   </si>
   <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
     <t xml:space="preserve">U22,U48,U49,U50,U51,U106,U107,U108,U109,U110,U146,U147,U148,U149,U150,U186,U187,U188,U189,U190</t>
   </si>
   <si>
@@ -187,9 +160,6 @@
     <t xml:space="preserve">4-Bit Magnitude Comparator</t>
   </si>
   <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
     <t xml:space="preserve">U23,U24,U25</t>
   </si>
   <si>
@@ -202,9 +172,6 @@
     <t xml:space="preserve">Synchronous 4-Bit Binary Counters</t>
   </si>
   <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
     <t xml:space="preserve">U27,U33,U34,U35,U53,U83,U84,U86,U124,U125,U126,U127,U164,U165,U166,U167</t>
   </si>
   <si>
@@ -220,9 +187,6 @@
     <t xml:space="preserve">Octal D-Type Transparent Latches with 3-state Outputs</t>
   </si>
   <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
     <t xml:space="preserve">U29,U30,U31,U32</t>
   </si>
   <si>
@@ -235,9 +199,6 @@
     <t xml:space="preserve">Quadruple 1-of-2 Data Selectors/Multiplexers</t>
   </si>
   <si>
-    <t xml:space="preserve">32</t>
-  </si>
-  <si>
     <t xml:space="preserve">U36,U37,U38,U39,U40,U41,U42,U59,U60,U61,U62,U87,U90,U92,U93,U94,U95,U96,U128,U131,U132,U133,U134,U135,U136,U168,U171,U172,U173,U174,U175,U176</t>
   </si>
   <si>
@@ -262,9 +223,6 @@
     <t xml:space="preserve">Dual Positive-Edge-Triggered D-Type Flip-Flops With Clear And Preset</t>
   </si>
   <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
     <t xml:space="preserve">U44,U45,U46,U47,U74,U75,U102,U103,U104,U105,U142,U143,U144,U145,U182,U183,U184,U185</t>
   </si>
   <si>
@@ -280,9 +238,6 @@
     <t xml:space="preserve">Quadruple 2-Input Positive-AND Gates</t>
   </si>
   <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
     <t xml:space="preserve">U54,U71,U112,U120,U152,U160,U192,U200</t>
   </si>
   <si>
@@ -415,9 +370,6 @@
     <t xml:space="preserve">SW-DIP8</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
     <t xml:space="preserve">EXPANSIONBUSP1,VIDEOP1</t>
   </si>
   <si>
@@ -485,6 +437,24 @@
   </si>
   <si>
     <t xml:space="preserve">64K (8Kx8) Static RAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One 100nF (0.1uF) capacitor for ICs marked with extra DC near pin 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K104K15X7RF53H5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.sg/ProductDetail/Vishay-BC-Components/K104K15X7RF53H5?qs=sYfpZ29HcUSlgH5bSUHkYw%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decoupling capacitors for each DC component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All with suffix CAP20</t>
   </si>
 </sst>
 </file>
@@ -584,25 +554,21 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="134.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="126.89"/>
@@ -637,893 +603,915 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AMH1" s="1"/>
-      <c r="AMI1" s="1"/>
-      <c r="AMJ1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="H2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="F3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="H3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="E4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="H4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="H5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="H6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>18</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>18</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>25</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="C9" s="0" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>59</v>
+        <v>18</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>16</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>18</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>65</v>
+        <v>18</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>70</v>
+        <v>18</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>32</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="F15" s="0" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>79</v>
+        <v>18</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>18</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>65</v>
+        <v>18</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>85</v>
+        <v>18</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="H19" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>85</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>85</v>
+        <v>18</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>18</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>39</v>
+        <v>18</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>65</v>
+        <v>18</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>18</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>39</v>
+        <v>101</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>39</v>
+        <v>101</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>54</v>
+        <v>101</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>129</v>
-      </c>
       <c r="H30" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>130</v>
+        <v>101</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>130</v>
+        <v>101</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>39</v>
+        <v>101</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>39</v>
+        <v>101</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>85</v>
+        <v>101</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>209</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A:H"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1531,6 +1519,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>